<commit_message>
Alguns erros de codigo e DSS
</commit_message>
<xml_diff>
--- a/Modelos UML/Descrição UseCases/Registar.xlsx
+++ b/Modelos UML/Descrição UseCases/Registar.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Luis\Documents\Luís\3º ano\1º Semestre\DSS\Trabalho\DSS\Modelos UML\Descrição UseCases\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pmcca\Documents\3º Ano\DSS\Trabalho\DSS\DSS\Modelos UML\Descrição UseCases\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{510D4FDA-43AE-4860-A5B7-51AC33B083AF}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4575"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4575" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>Actor input</t>
   </si>
@@ -72,41 +73,44 @@
     <t>4. Apresenta dados pessoais</t>
   </si>
   <si>
-    <t>5. Regista cliente</t>
-  </si>
-  <si>
-    <t>5.1. Informa cliente que já está registado</t>
-  </si>
-  <si>
-    <t>5.1.1. Informa cliente que os dados são inválidos</t>
-  </si>
-  <si>
-    <t>6. Informa cliente de que foi registado</t>
-  </si>
-  <si>
     <t>Regressa a 4</t>
   </si>
   <si>
-    <t>5.2. Sai do ecrã de registo</t>
+    <t>Regressa a 1</t>
+  </si>
+  <si>
+    <t>5. Verifica Dados</t>
+  </si>
+  <si>
+    <t>6. Regista Cliente</t>
+  </si>
+  <si>
+    <t>7. Informa cliente de que foi registado com sucesso</t>
   </si>
   <si>
     <t>Alternativa 1
 [Cliente já registado]
-(Passo 5)</t>
+(Passo 6)</t>
+  </si>
+  <si>
+    <t>6.1. Informa cliente que já está registado</t>
+  </si>
+  <si>
+    <t>6.2. Sai do ecrã de registo</t>
   </si>
   <si>
     <t>Alternativa 2
 [Dados inválidos]
-(Passo 5)</t>
-  </si>
-  <si>
-    <t>Regressa a 1</t>
+(Passo 6)</t>
+  </si>
+  <si>
+    <t>6.1.1. Informa cliente que os dados são inválidos</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -707,11 +711,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:D19"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -802,7 +806,7 @@
       <c r="B11" s="26"/>
       <c r="C11" s="4"/>
       <c r="D11" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="12" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
@@ -815,45 +819,47 @@
     <row r="13" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B13" s="26"/>
       <c r="C13" s="4"/>
-      <c r="D13" s="1"/>
+      <c r="D13" s="1" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="14" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B14" s="19" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C14" s="3"/>
       <c r="D14" s="2" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
     </row>
     <row r="15" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B15" s="20"/>
       <c r="C15" s="4"/>
       <c r="D15" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="16" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B16" s="20"/>
       <c r="C16" s="4"/>
       <c r="D16" s="1" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
     </row>
     <row r="17" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B17" s="16" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C17" s="6"/>
       <c r="D17" s="13" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
     </row>
     <row r="18" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B18" s="17"/>
       <c r="C18" s="9"/>
       <c r="D18" s="11" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="19" spans="2:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">

</xml_diff>